<commit_message>
system logs and upload format
</commit_message>
<xml_diff>
--- a/public/assets/SMS Activity Plan Upload Format.xlsx
+++ b/public/assets/SMS Activity Plan Upload Format.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2E8E99-AF27-41B1-BBC3-084796CB6517}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8E2B13-2CCC-4A08-85D3-001D6AF0BED3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="127">
   <si>
     <t>YEAR</t>
   </si>
@@ -93,9 +93,6 @@
     <t>MAKATI</t>
   </si>
   <si>
-    <t>QUEZON CITY</t>
-  </si>
-  <si>
     <t>WORK WITH</t>
   </si>
   <si>
@@ -435,151 +432,10 @@
     <t>GROUP CODE</t>
   </si>
   <si>
-    <t>ADMIN &amp; ALIGNMENT W/ OTHER DEPARTMENT</t>
-  </si>
-  <si>
-    <t>PGJR-727</t>
-  </si>
-  <si>
-    <t>MANILA</t>
-  </si>
-  <si>
-    <t>STORE VISIT &amp; WORK WITH</t>
-  </si>
-  <si>
-    <t>PPCI-132</t>
-  </si>
-  <si>
-    <t>PPCI-145</t>
-  </si>
-  <si>
-    <t>PPCI-102</t>
-  </si>
-  <si>
-    <t>PPCI-316</t>
-  </si>
-  <si>
-    <t>PASAY</t>
-  </si>
-  <si>
-    <t>ADMIN OF PPCI BR PRESENTATION (PASAY ADMIN)</t>
-  </si>
-  <si>
-    <t>ADMIN OF PPCI BR PRESENTATION (MANILA ADMIN)</t>
-  </si>
-  <si>
-    <t>REMITTANCE, ALIGNMENT</t>
-  </si>
-  <si>
-    <t>HEAD OFFICE COLLECTION (MERRYMART)</t>
-  </si>
-  <si>
-    <t>HEAD OFFICE COLLECTION &amp; ALIGNMENT (PUREMART)</t>
-  </si>
-  <si>
-    <t>PPCI-HO-1</t>
-  </si>
-  <si>
-    <t>BR SCHEDULE</t>
-  </si>
-  <si>
-    <t>PGJR-735</t>
-  </si>
-  <si>
-    <t>STORE VISIT AND VALIDATION OF NEW MERCHANDISER DEPLOYMENT</t>
-  </si>
-  <si>
-    <t>PPCI-112</t>
-  </si>
-  <si>
-    <t>PPCI-137</t>
-  </si>
-  <si>
-    <t>PPCI-115</t>
-  </si>
-  <si>
-    <t>PPCI-108</t>
-  </si>
-  <si>
-    <t>PPCI-111</t>
-  </si>
-  <si>
-    <t>PPCI-118</t>
-  </si>
-  <si>
-    <t>STORE VISIT AND VALIDATION OF NEW MERCHANDISER</t>
-  </si>
-  <si>
-    <t>PPCI-134</t>
-  </si>
-  <si>
-    <t>PPCI-135</t>
-  </si>
-  <si>
-    <t>PGJR-726</t>
-  </si>
-  <si>
-    <t>CAVITE</t>
-  </si>
-  <si>
-    <t>PPCI-141</t>
-  </si>
-  <si>
-    <t>PPCI-267</t>
-  </si>
-  <si>
-    <t>PPCI-397</t>
-  </si>
-  <si>
-    <t>PPCI-353</t>
-  </si>
-  <si>
-    <t>RECON</t>
-  </si>
-  <si>
-    <t>PGJR-297</t>
-  </si>
-  <si>
-    <t>VALENZUELA</t>
-  </si>
-  <si>
-    <t>STORE VISIT AND VALIDATION OF NEW MERCHANDISER, WORK WITH</t>
-  </si>
-  <si>
-    <t>PPCI-138</t>
-  </si>
-  <si>
-    <t>PPCI-105</t>
-  </si>
-  <si>
-    <t>STORE VISIT AND VALIDATION OF NEW MERCHANDISER, WORK WITH (GEN. T DE LEON)</t>
-  </si>
-  <si>
-    <t>ADMIN, REMITTANCE</t>
-  </si>
-  <si>
-    <t>HEAD OFFICE COLLECTION (PUREMART)</t>
-  </si>
-  <si>
-    <t>DAVAO</t>
-  </si>
-  <si>
-    <t>STORE VISIT, PROVINCIAL VISIT (SMC DAVAO BANGKAL)</t>
-  </si>
-  <si>
-    <t>STORE VISIT, PROVINCIAL VISIT (SVI MATINA DAVAO)</t>
-  </si>
-  <si>
-    <t>OPENING MERRYMART DAVAO</t>
-  </si>
-  <si>
-    <t>STORE VISIT, PROVINCIAL VISIT (ROBINSONS ABREEZA)</t>
-  </si>
-  <si>
-    <t>STORE VISIT, PROVINCIAL VISIT (SMC BAJADA)</t>
-  </si>
-  <si>
     <t>FIRSTNAME</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
   </si>
 </sst>
 </file>
@@ -690,7 +546,30 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -969,7 +848,7 @@
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,16 +918,16 @@
         <v>7</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1059,9 +938,15 @@
         <v>44958</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="G5" s="5"/>
       <c r="H5" t="str">
         <f>IFERROR(VLOOKUP(G5, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
@@ -1089,18 +974,6 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
-      <c r="H6" t="str">
-        <f>IFERROR(VLOOKUP(G6, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I6" t="str">
-        <f>IFERROR(VLOOKUP(G6, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J6" t="str">
-        <f>IFERROR(VLOOKUP(G6, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1111,22 +984,10 @@
         <v>44960</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
-      <c r="H7" t="str">
-        <f>IFERROR(VLOOKUP(G7, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I7" t="str">
-        <f>IFERROR(VLOOKUP(G7, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J7" t="str">
-        <f>IFERROR(VLOOKUP(G7, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1141,18 +1002,6 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
-      <c r="H8" t="str">
-        <f>IFERROR(VLOOKUP(G8, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I8" t="str">
-        <f>IFERROR(VLOOKUP(G8, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J8" t="str">
-        <f>IFERROR(VLOOKUP(G8, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1167,18 +1016,6 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
-      <c r="H9" t="str">
-        <f>IFERROR(VLOOKUP(G9, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I9" t="str">
-        <f>IFERROR(VLOOKUP(G9, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J9" t="str">
-        <f>IFERROR(VLOOKUP(G9, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1189,30 +1026,10 @@
         <v>44963</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" t="str">
-        <f>IFERROR(VLOOKUP(G10, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v>Herbert</v>
-      </c>
-      <c r="I10" t="str">
-        <f>IFERROR(VLOOKUP(G10, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v>Rodriguez</v>
-      </c>
-      <c r="J10" t="str">
-        <f>IFERROR(VLOOKUP(G10, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v>NKA</v>
-      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1223,27 +1040,9 @@
         <v>44964</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H11" t="str">
-        <f>IFERROR(VLOOKUP(G11, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I11" t="str">
-        <f>IFERROR(VLOOKUP(G11, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J11" t="str">
-        <f>IFERROR(VLOOKUP(G11, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1254,27 +1053,9 @@
         <v>44964</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H12" t="str">
-        <f>IFERROR(VLOOKUP(G12, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I12" t="str">
-        <f>IFERROR(VLOOKUP(G12, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J12" t="str">
-        <f>IFERROR(VLOOKUP(G12, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1285,27 +1066,9 @@
         <v>44964</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H13" t="str">
-        <f>IFERROR(VLOOKUP(G13, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I13" t="str">
-        <f>IFERROR(VLOOKUP(G13, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J13" t="str">
-        <f>IFERROR(VLOOKUP(G13, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1316,27 +1079,9 @@
         <v>44964</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H14" t="str">
-        <f>IFERROR(VLOOKUP(G14, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I14" t="str">
-        <f>IFERROR(VLOOKUP(G14, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J14" t="str">
-        <f>IFERROR(VLOOKUP(G14, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1347,27 +1092,9 @@
         <v>44964</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H15" t="str">
-        <f>IFERROR(VLOOKUP(G15, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I15" t="str">
-        <f>IFERROR(VLOOKUP(G15, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J15" t="str">
-        <f>IFERROR(VLOOKUP(G15, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1378,28 +1105,10 @@
         <v>44965</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>135</v>
-      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="5"/>
-      <c r="H16" t="str">
-        <f>IFERROR(VLOOKUP(G16, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I16" t="str">
-        <f>IFERROR(VLOOKUP(G16, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J16" t="str">
-        <f>IFERROR(VLOOKUP(G16, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1410,28 +1119,10 @@
         <v>44966</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>136</v>
-      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="5"/>
-      <c r="H17" t="str">
-        <f>IFERROR(VLOOKUP(G17, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I17" t="str">
-        <f>IFERROR(VLOOKUP(G17, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J17" t="str">
-        <f>IFERROR(VLOOKUP(G17, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1442,28 +1133,10 @@
         <v>44967</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>137</v>
-      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="5"/>
-      <c r="H18" t="str">
-        <f>IFERROR(VLOOKUP(G18, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I18" t="str">
-        <f>IFERROR(VLOOKUP(G18, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J18" t="str">
-        <f>IFERROR(VLOOKUP(G18, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1474,28 +1147,10 @@
         <v>44967</v>
       </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>138</v>
-      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="5"/>
-      <c r="H19" t="str">
-        <f>IFERROR(VLOOKUP(G19, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I19" t="str">
-        <f>IFERROR(VLOOKUP(G19, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J19" t="str">
-        <f>IFERROR(VLOOKUP(G19, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1506,28 +1161,10 @@
         <v>44967</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>139</v>
-      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="5"/>
-      <c r="H20" t="str">
-        <f>IFERROR(VLOOKUP(G20, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I20" t="str">
-        <f>IFERROR(VLOOKUP(G20, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J20" t="str">
-        <f>IFERROR(VLOOKUP(G20, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1541,18 +1178,6 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" t="str">
-        <f>IFERROR(VLOOKUP(G21, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I21" t="str">
-        <f>IFERROR(VLOOKUP(G21, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J21" t="str">
-        <f>IFERROR(VLOOKUP(G21, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1566,18 +1191,6 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" t="str">
-        <f>IFERROR(VLOOKUP(G22, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I22" t="str">
-        <f>IFERROR(VLOOKUP(G22, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J22" t="str">
-        <f>IFERROR(VLOOKUP(G22, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1588,28 +1201,10 @@
         <v>44970</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>126</v>
-      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="5"/>
-      <c r="H23" t="str">
-        <f>IFERROR(VLOOKUP(G23, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I23" t="str">
-        <f>IFERROR(VLOOKUP(G23, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J23" t="str">
-        <f>IFERROR(VLOOKUP(G23, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1620,28 +1215,10 @@
         <v>44971</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>141</v>
-      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="6"/>
       <c r="G24" s="5"/>
-      <c r="H24" t="str">
-        <f>IFERROR(VLOOKUP(G24, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I24" t="str">
-        <f>IFERROR(VLOOKUP(G24, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J24" t="str">
-        <f>IFERROR(VLOOKUP(G24, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K24" s="10"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1652,28 +1229,10 @@
         <v>44972</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>143</v>
-      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="6"/>
       <c r="G25" s="5"/>
-      <c r="H25" t="str">
-        <f>IFERROR(VLOOKUP(G25, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I25" t="str">
-        <f>IFERROR(VLOOKUP(G25, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J25" t="str">
-        <f>IFERROR(VLOOKUP(G25, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K25" s="10"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1684,28 +1243,10 @@
         <v>44972</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>143</v>
-      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="5"/>
-      <c r="H26" t="str">
-        <f>IFERROR(VLOOKUP(G26, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I26" t="str">
-        <f>IFERROR(VLOOKUP(G26, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J26" t="str">
-        <f>IFERROR(VLOOKUP(G26, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1716,28 +1257,10 @@
         <v>44972</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>143</v>
-      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="5"/>
-      <c r="H27" t="str">
-        <f>IFERROR(VLOOKUP(G27, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I27" t="str">
-        <f>IFERROR(VLOOKUP(G27, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J27" t="str">
-        <f>IFERROR(VLOOKUP(G27, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1748,28 +1271,10 @@
         <v>44972</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>143</v>
-      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="5"/>
-      <c r="H28" t="str">
-        <f>IFERROR(VLOOKUP(G28, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I28" t="str">
-        <f>IFERROR(VLOOKUP(G28, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J28" t="str">
-        <f>IFERROR(VLOOKUP(G28, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1780,28 +1285,10 @@
         <v>44972</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>143</v>
-      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
       <c r="G29" s="5"/>
-      <c r="H29" t="str">
-        <f>IFERROR(VLOOKUP(G29, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I29" t="str">
-        <f>IFERROR(VLOOKUP(G29, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J29" t="str">
-        <f>IFERROR(VLOOKUP(G29, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1812,28 +1299,10 @@
         <v>44973</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>143</v>
-      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
       <c r="G30" s="5"/>
-      <c r="H30" t="str">
-        <f>IFERROR(VLOOKUP(G30, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I30" t="str">
-        <f>IFERROR(VLOOKUP(G30, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J30" t="str">
-        <f>IFERROR(VLOOKUP(G30, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K30" s="10"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1844,28 +1313,10 @@
         <v>44973</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>150</v>
-      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
       <c r="G31" s="5"/>
-      <c r="H31" t="str">
-        <f>IFERROR(VLOOKUP(G31, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I31" t="str">
-        <f>IFERROR(VLOOKUP(G31, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J31" t="str">
-        <f>IFERROR(VLOOKUP(G31, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1876,28 +1327,10 @@
         <v>44973</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>150</v>
-      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
       <c r="G32" s="5"/>
-      <c r="H32" t="str">
-        <f>IFERROR(VLOOKUP(G32, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I32" t="str">
-        <f>IFERROR(VLOOKUP(G32, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J32" t="str">
-        <f>IFERROR(VLOOKUP(G32, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K32" s="10"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1908,28 +1341,10 @@
         <v>44973</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>150</v>
-      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
       <c r="G33" s="5"/>
-      <c r="H33" t="str">
-        <f>IFERROR(VLOOKUP(G33, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I33" t="str">
-        <f>IFERROR(VLOOKUP(G33, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J33" t="str">
-        <f>IFERROR(VLOOKUP(G33, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K33" s="10"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1940,28 +1355,10 @@
         <v>44974</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>143</v>
-      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
       <c r="G34" s="5"/>
-      <c r="H34" t="str">
-        <f>IFERROR(VLOOKUP(G34, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I34" t="str">
-        <f>IFERROR(VLOOKUP(G34, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J34" t="str">
-        <f>IFERROR(VLOOKUP(G34, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1972,28 +1369,10 @@
         <v>44974</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>138</v>
-      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
       <c r="G35" s="5"/>
-      <c r="H35" t="str">
-        <f>IFERROR(VLOOKUP(G35, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I35" t="str">
-        <f>IFERROR(VLOOKUP(G35, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J35" t="str">
-        <f>IFERROR(VLOOKUP(G35, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K35" s="10"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2004,28 +1383,10 @@
         <v>44974</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>139</v>
-      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
       <c r="G36" s="5"/>
-      <c r="H36" t="str">
-        <f>IFERROR(VLOOKUP(G36, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I36" t="str">
-        <f>IFERROR(VLOOKUP(G36, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J36" t="str">
-        <f>IFERROR(VLOOKUP(G36, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K36" s="10"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2039,18 +1400,6 @@
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="G37" s="5"/>
-      <c r="H37" t="str">
-        <f>IFERROR(VLOOKUP(G37, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I37" t="str">
-        <f>IFERROR(VLOOKUP(G37, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J37" t="str">
-        <f>IFERROR(VLOOKUP(G37, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K37" s="10"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2064,18 +1413,6 @@
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" t="str">
-        <f>IFERROR(VLOOKUP(G38, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I38" t="str">
-        <f>IFERROR(VLOOKUP(G38, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J38" t="str">
-        <f>IFERROR(VLOOKUP(G38, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K38" s="10"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2086,28 +1423,10 @@
         <v>44977</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>126</v>
-      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
       <c r="G39" s="5"/>
-      <c r="H39" t="str">
-        <f>IFERROR(VLOOKUP(G39, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I39" t="str">
-        <f>IFERROR(VLOOKUP(G39, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J39" t="str">
-        <f>IFERROR(VLOOKUP(G39, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K39" s="10"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2118,28 +1437,10 @@
         <v>44978</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>150</v>
-      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
       <c r="G40" s="5"/>
-      <c r="H40" t="str">
-        <f>IFERROR(VLOOKUP(G40, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I40" t="str">
-        <f>IFERROR(VLOOKUP(G40, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J40" t="str">
-        <f>IFERROR(VLOOKUP(G40, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K40" s="10"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2150,28 +1451,10 @@
         <v>44978</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>150</v>
-      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
       <c r="G41" s="5"/>
-      <c r="H41" t="str">
-        <f>IFERROR(VLOOKUP(G41, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I41" t="str">
-        <f>IFERROR(VLOOKUP(G41, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J41" t="str">
-        <f>IFERROR(VLOOKUP(G41, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K41" s="10"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2182,28 +1465,10 @@
         <v>44978</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>150</v>
-      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
       <c r="G42" s="5"/>
-      <c r="H42" t="str">
-        <f>IFERROR(VLOOKUP(G42, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I42" t="str">
-        <f>IFERROR(VLOOKUP(G42, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J42" t="str">
-        <f>IFERROR(VLOOKUP(G42, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K42" s="10"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2214,28 +1479,10 @@
         <v>44978</v>
       </c>
       <c r="C43" s="5"/>
-      <c r="D43" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>150</v>
-      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
       <c r="G43" s="5"/>
-      <c r="H43" t="str">
-        <f>IFERROR(VLOOKUP(G43, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I43" t="str">
-        <f>IFERROR(VLOOKUP(G43, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J43" t="str">
-        <f>IFERROR(VLOOKUP(G43, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K43" s="10"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2246,28 +1493,10 @@
         <v>44978</v>
       </c>
       <c r="C44" s="5"/>
-      <c r="D44" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>150</v>
-      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
       <c r="G44" s="5"/>
-      <c r="H44" t="str">
-        <f>IFERROR(VLOOKUP(G44, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I44" t="str">
-        <f>IFERROR(VLOOKUP(G44, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J44" t="str">
-        <f>IFERROR(VLOOKUP(G44, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K44" s="10"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2278,28 +1507,9 @@
         <v>44979</v>
       </c>
       <c r="C45" s="5"/>
-      <c r="D45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>159</v>
-      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="2"/>
       <c r="G45" s="5"/>
-      <c r="H45" t="str">
-        <f>IFERROR(VLOOKUP(G45, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I45" t="str">
-        <f>IFERROR(VLOOKUP(G45, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J45" t="str">
-        <f>IFERROR(VLOOKUP(G45, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K45" s="10"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2310,30 +1520,9 @@
         <v>44980</v>
       </c>
       <c r="C46" s="5"/>
-      <c r="D46" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G46" t="s">
-        <v>113</v>
-      </c>
-      <c r="H46" t="str">
-        <f>IFERROR(VLOOKUP(G46, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v>Ronelo</v>
-      </c>
-      <c r="I46" t="str">
-        <f>IFERROR(VLOOKUP(G46, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v>Ordiz</v>
-      </c>
-      <c r="J46" t="str">
-        <f>IFERROR(VLOOKUP(G46, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v>RD</v>
-      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
       <c r="K46" s="10"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2344,30 +1533,9 @@
         <v>44980</v>
       </c>
       <c r="C47" s="5"/>
-      <c r="D47" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G47" t="s">
-        <v>116</v>
-      </c>
-      <c r="H47" t="str">
-        <f>IFERROR(VLOOKUP(G47, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v>Ruby</v>
-      </c>
-      <c r="I47" t="str">
-        <f>IFERROR(VLOOKUP(G47, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v>Salud</v>
-      </c>
-      <c r="J47" t="str">
-        <f>IFERROR(VLOOKUP(G47, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v>CMD</v>
-      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
       <c r="K47" s="10"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2378,30 +1546,9 @@
         <v>44980</v>
       </c>
       <c r="C48" s="5"/>
-      <c r="D48" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G48" t="s">
-        <v>122</v>
-      </c>
-      <c r="H48" t="str">
-        <f>IFERROR(VLOOKUP(G48, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v>Jelou</v>
-      </c>
-      <c r="I48" t="str">
-        <f>IFERROR(VLOOKUP(G48, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v>Cabuga</v>
-      </c>
-      <c r="J48" t="str">
-        <f>IFERROR(VLOOKUP(G48, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v>RD</v>
-      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
       <c r="K48" s="10"/>
     </row>
     <row r="49" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2412,30 +1559,9 @@
         <v>44980</v>
       </c>
       <c r="C49" s="5"/>
-      <c r="D49" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G49" t="s">
-        <v>116</v>
-      </c>
-      <c r="H49" t="str">
-        <f>IFERROR(VLOOKUP(G49, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v>Ruby</v>
-      </c>
-      <c r="I49" t="str">
-        <f>IFERROR(VLOOKUP(G49, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v>Salud</v>
-      </c>
-      <c r="J49" t="str">
-        <f>IFERROR(VLOOKUP(G49, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v>CMD</v>
-      </c>
+      <c r="D49" s="4"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
       <c r="K49" s="10"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2446,28 +1572,10 @@
         <v>44981</v>
       </c>
       <c r="C50" s="5"/>
-      <c r="D50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
       <c r="G50" s="5"/>
-      <c r="H50" t="str">
-        <f>IFERROR(VLOOKUP(G50, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I50" t="str">
-        <f>IFERROR(VLOOKUP(G50, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J50" t="str">
-        <f>IFERROR(VLOOKUP(G50, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K50" s="10"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2478,28 +1586,10 @@
         <v>44981</v>
       </c>
       <c r="C51" s="5"/>
-      <c r="D51" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>138</v>
-      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
       <c r="G51" s="5"/>
-      <c r="H51" t="str">
-        <f>IFERROR(VLOOKUP(G51, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I51" t="str">
-        <f>IFERROR(VLOOKUP(G51, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J51" t="str">
-        <f>IFERROR(VLOOKUP(G51, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K51" s="10"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2510,28 +1600,10 @@
         <v>44981</v>
       </c>
       <c r="C52" s="5"/>
-      <c r="D52" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>167</v>
-      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
       <c r="G52" s="5"/>
-      <c r="H52" t="str">
-        <f>IFERROR(VLOOKUP(G52, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I52" t="str">
-        <f>IFERROR(VLOOKUP(G52, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J52" t="str">
-        <f>IFERROR(VLOOKUP(G52, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K52" s="10"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2545,18 +1617,6 @@
       <c r="D53" s="4"/>
       <c r="E53" s="5"/>
       <c r="G53" s="5"/>
-      <c r="H53" t="str">
-        <f>IFERROR(VLOOKUP(G53, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I53" t="str">
-        <f>IFERROR(VLOOKUP(G53, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J53" t="str">
-        <f>IFERROR(VLOOKUP(G53, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K53" s="10"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2570,18 +1630,6 @@
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="G54" s="5"/>
-      <c r="H54" t="str">
-        <f>IFERROR(VLOOKUP(G54, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I54" t="str">
-        <f>IFERROR(VLOOKUP(G54, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J54" t="str">
-        <f>IFERROR(VLOOKUP(G54, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K54" s="10"/>
     </row>
     <row r="55" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2592,28 +1640,10 @@
         <v>44984</v>
       </c>
       <c r="C55" s="5"/>
-      <c r="D55" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>169</v>
-      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
       <c r="G55" s="5"/>
-      <c r="H55" t="str">
-        <f>IFERROR(VLOOKUP(G55, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I55" t="str">
-        <f>IFERROR(VLOOKUP(G55, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J55" t="str">
-        <f>IFERROR(VLOOKUP(G55, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K55" s="10"/>
     </row>
     <row r="56" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2624,28 +1654,10 @@
         <v>44984</v>
       </c>
       <c r="C56" s="5"/>
-      <c r="D56" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>170</v>
-      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
       <c r="G56" s="5"/>
-      <c r="H56" t="str">
-        <f>IFERROR(VLOOKUP(G56, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I56" t="str">
-        <f>IFERROR(VLOOKUP(G56, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J56" t="str">
-        <f>IFERROR(VLOOKUP(G56, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K56" s="10"/>
     </row>
     <row r="57" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2656,28 +1668,10 @@
         <v>44985</v>
       </c>
       <c r="C57" s="5"/>
-      <c r="D57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>171</v>
-      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
       <c r="G57" s="5"/>
-      <c r="H57" t="str">
-        <f>IFERROR(VLOOKUP(G57, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I57" t="str">
-        <f>IFERROR(VLOOKUP(G57, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J57" t="str">
-        <f>IFERROR(VLOOKUP(G57, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K57" s="10"/>
     </row>
     <row r="58" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2688,28 +1682,10 @@
         <v>44985</v>
       </c>
       <c r="C58" s="5"/>
-      <c r="D58" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>172</v>
-      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
       <c r="G58" s="5"/>
-      <c r="H58" t="str">
-        <f>IFERROR(VLOOKUP(G58, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I58" t="str">
-        <f>IFERROR(VLOOKUP(G58, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J58" t="str">
-        <f>IFERROR(VLOOKUP(G58, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K58" s="10"/>
     </row>
     <row r="59" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2720,28 +1696,10 @@
         <v>44985</v>
       </c>
       <c r="C59" s="5"/>
-      <c r="D59" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>173</v>
-      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
       <c r="G59" s="5"/>
-      <c r="H59" t="str">
-        <f>IFERROR(VLOOKUP(G59, 'WORK WITH USERS'!$A$2:$D$38, 2, 1), "")</f>
-        <v/>
-      </c>
-      <c r="I59" t="str">
-        <f>IFERROR(VLOOKUP(G59, 'WORK WITH USERS'!$A$2:$D$38, 3, 1), "")</f>
-        <v/>
-      </c>
-      <c r="J59" t="str">
-        <f>IFERROR(VLOOKUP(G59, 'WORK WITH USERS'!$A$2:$D$38, 4, 1), "")</f>
-        <v/>
-      </c>
       <c r="K59" s="10"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2796,534 +1754,534 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
       <c r="D1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
       <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
       <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
         <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s">
-        <v>48</v>
-      </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
-        <v>54</v>
-      </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
         <v>55</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="C15" t="s">
-        <v>57</v>
-      </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
         <v>58</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>59</v>
       </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
         <v>61</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>62</v>
       </c>
-      <c r="C17" t="s">
-        <v>63</v>
-      </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>65</v>
       </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
         <v>67</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>68</v>
       </c>
-      <c r="C19" t="s">
-        <v>69</v>
-      </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
         <v>70</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>71</v>
       </c>
-      <c r="C20" t="s">
-        <v>72</v>
-      </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
         <v>71</v>
       </c>
-      <c r="C21" t="s">
-        <v>72</v>
-      </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
         <v>74</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>75</v>
       </c>
-      <c r="C22" t="s">
-        <v>76</v>
-      </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
         <v>77</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>78</v>
       </c>
-      <c r="C23" t="s">
-        <v>79</v>
-      </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
         <v>80</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>81</v>
       </c>
-      <c r="C24" t="s">
-        <v>82</v>
-      </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
         <v>83</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>84</v>
       </c>
-      <c r="C25" t="s">
-        <v>85</v>
-      </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
         <v>86</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>87</v>
       </c>
-      <c r="C26" t="s">
-        <v>88</v>
-      </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
         <v>89</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>90</v>
       </c>
-      <c r="C27" t="s">
-        <v>91</v>
-      </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
         <v>92</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>93</v>
       </c>
-      <c r="C28" t="s">
-        <v>94</v>
-      </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
         <v>95</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>96</v>
       </c>
-      <c r="C29" t="s">
-        <v>97</v>
-      </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
         <v>98</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>99</v>
       </c>
-      <c r="C30" t="s">
-        <v>100</v>
-      </c>
       <c r="D30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
         <v>101</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>102</v>
       </c>
-      <c r="C31" t="s">
-        <v>103</v>
-      </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
         <v>104</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>105</v>
       </c>
-      <c r="C32" t="s">
-        <v>106</v>
-      </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" t="s">
         <v>107</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>108</v>
       </c>
-      <c r="C33" t="s">
-        <v>109</v>
-      </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" t="s">
         <v>110</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>111</v>
       </c>
-      <c r="C34" t="s">
-        <v>112</v>
-      </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" t="s">
         <v>113</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>114</v>
       </c>
-      <c r="C35" t="s">
-        <v>115</v>
-      </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
         <v>116</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>117</v>
       </c>
-      <c r="C36" t="s">
-        <v>118</v>
-      </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" t="s">
         <v>119</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>120</v>
       </c>
-      <c r="C37" t="s">
-        <v>121</v>
-      </c>
       <c r="D37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" t="s">
         <v>122</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>123</v>
       </c>
-      <c r="C38" t="s">
-        <v>124</v>
-      </c>
       <c r="D38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
branch restriction, org structure, and schedule displays
</commit_message>
<xml_diff>
--- a/public/assets/SMS Activity Plan Upload Format.xlsx
+++ b/public/assets/SMS Activity Plan Upload Format.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730F5BC0-F207-4C72-9B43-9269DD1889F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93317E5-3BEB-475D-96CC-1D8408AC3B1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,6 +25,30 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{7FFE30EF-0A42-4D3A-81A1-2CF69EEBAF6C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Day of the month must be between 1 to 31.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D4" authorId="0" shapeId="0" xr:uid="{678EBF7D-FFE9-4211-9DA8-D61524758890}">
       <text>
         <r>
@@ -108,9 +132,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="ddd"/>
     <numFmt numFmtId="165" formatCode="dddd"/>
-    <numFmt numFmtId="168" formatCode="[$-3409]dddd\,\ mmmm\ dd\,\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-3409]dddd\,\ mmmm\ dd\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +182,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -437,7 +474,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -813,7 +850,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +939,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A5&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" ref="B5:B36" si="0">TEXT($B$2&amp;"/"&amp;A5&amp;"/"&amp;$B$1, "ddd")</f>
         <v>Tue</v>
       </c>
       <c r="C5" s="9"/>
@@ -924,7 +961,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A6&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C6" s="12"/>
@@ -938,7 +975,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A7&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C7" s="12"/>
@@ -952,7 +989,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A8&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C8" s="12"/>
@@ -966,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A9&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C9" s="12"/>
@@ -980,7 +1017,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A10&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C10" s="12"/>
@@ -994,7 +1031,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A11&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C11" s="12"/>
@@ -1008,7 +1045,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A12&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
       <c r="C12" s="12"/>
@@ -1022,7 +1059,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A13&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
       <c r="C13" s="12"/>
@@ -1036,7 +1073,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A14&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
       <c r="C14" s="12"/>
@@ -1050,7 +1087,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A15&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
       <c r="C15" s="12"/>
@@ -1064,7 +1101,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A16&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="C16" s="12"/>
@@ -1078,7 +1115,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A17&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="C17" s="12"/>
@@ -1092,7 +1129,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A18&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="C18" s="12"/>
@@ -1106,7 +1143,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A19&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="C19" s="12"/>
@@ -1120,7 +1157,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A20&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="C20" s="12"/>
@@ -1134,7 +1171,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A21&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="C21" s="12"/>
@@ -1148,7 +1185,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A22&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="C22" s="12"/>
@@ -1162,7 +1199,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A23&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
       <c r="C23" s="12"/>
@@ -1176,7 +1213,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A24&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C24" s="12"/>
@@ -1190,7 +1227,7 @@
         <v>10</v>
       </c>
       <c r="B25" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A25&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C25" s="12"/>
@@ -1204,7 +1241,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A26&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C26" s="12"/>
@@ -1218,7 +1255,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A27&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C27" s="12"/>
@@ -1232,7 +1269,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A28&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C28" s="12"/>
@@ -1246,7 +1283,7 @@
         <v>10</v>
       </c>
       <c r="B29" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A29&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="C29" s="12"/>
@@ -1260,7 +1297,7 @@
         <v>11</v>
       </c>
       <c r="B30" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A30&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
       <c r="C30" s="12"/>
@@ -1274,7 +1311,7 @@
         <v>12</v>
       </c>
       <c r="B31" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A31&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="C31" s="12"/>
@@ -1288,7 +1325,7 @@
         <v>15</v>
       </c>
       <c r="B32" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A32&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="C32" s="12"/>
@@ -1302,7 +1339,7 @@
         <v>16</v>
       </c>
       <c r="B33" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A33&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
       <c r="C33" s="12"/>
@@ -1316,7 +1353,7 @@
         <v>16</v>
       </c>
       <c r="B34" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A34&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
       <c r="C34" s="12"/>
@@ -1330,7 +1367,7 @@
         <v>16</v>
       </c>
       <c r="B35" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A35&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
       <c r="C35" s="12"/>
@@ -1344,7 +1381,7 @@
         <v>16</v>
       </c>
       <c r="B36" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A36&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
       <c r="C36" s="12"/>
@@ -1358,7 +1395,7 @@
         <v>16</v>
       </c>
       <c r="B37" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A37&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" ref="B37:B68" si="1">TEXT($B$2&amp;"/"&amp;A37&amp;"/"&amp;$B$1, "ddd")</f>
         <v>Tue</v>
       </c>
       <c r="C37" s="12"/>
@@ -1372,7 +1409,7 @@
         <v>16</v>
       </c>
       <c r="B38" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A38&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Tue</v>
       </c>
       <c r="C38" s="12"/>
@@ -1386,7 +1423,7 @@
         <v>17</v>
       </c>
       <c r="B39" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A39&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Wed</v>
       </c>
       <c r="C39" s="12"/>
@@ -1400,7 +1437,7 @@
         <v>17</v>
       </c>
       <c r="B40" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A40&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Wed</v>
       </c>
       <c r="C40" s="12"/>
@@ -1414,7 +1451,7 @@
         <v>17</v>
       </c>
       <c r="B41" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A41&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Wed</v>
       </c>
       <c r="C41" s="12"/>
@@ -1428,7 +1465,7 @@
         <v>18</v>
       </c>
       <c r="B42" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A42&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Thu</v>
       </c>
       <c r="C42" s="12"/>
@@ -1442,7 +1479,7 @@
         <v>18</v>
       </c>
       <c r="B43" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A43&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Thu</v>
       </c>
       <c r="C43" s="12"/>
@@ -1456,7 +1493,7 @@
         <v>18</v>
       </c>
       <c r="B44" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A44&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Thu</v>
       </c>
       <c r="C44" s="12"/>
@@ -1470,7 +1507,7 @@
         <v>18</v>
       </c>
       <c r="B45" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A45&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Thu</v>
       </c>
       <c r="C45" s="12"/>
@@ -1484,7 +1521,7 @@
         <v>19</v>
       </c>
       <c r="B46" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A46&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Fri</v>
       </c>
       <c r="C46" s="12"/>
@@ -1498,7 +1535,7 @@
         <v>19</v>
       </c>
       <c r="B47" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A47&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Fri</v>
       </c>
       <c r="C47" s="12"/>
@@ -1512,7 +1549,7 @@
         <v>19</v>
       </c>
       <c r="B48" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A48&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Fri</v>
       </c>
       <c r="C48" s="12"/>
@@ -1526,7 +1563,7 @@
         <v>22</v>
       </c>
       <c r="B49" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A49&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Mon</v>
       </c>
       <c r="C49" s="12"/>
@@ -1540,7 +1577,7 @@
         <v>22</v>
       </c>
       <c r="B50" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A50&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Mon</v>
       </c>
       <c r="C50" s="12"/>
@@ -1554,7 +1591,7 @@
         <v>22</v>
       </c>
       <c r="B51" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A51&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Mon</v>
       </c>
       <c r="C51" s="12"/>
@@ -1568,7 +1605,7 @@
         <v>22</v>
       </c>
       <c r="B52" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A52&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Mon</v>
       </c>
       <c r="C52" s="12"/>
@@ -1582,7 +1619,7 @@
         <v>23</v>
       </c>
       <c r="B53" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A53&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Tue</v>
       </c>
       <c r="C53" s="12"/>
@@ -1596,7 +1633,7 @@
         <v>24</v>
       </c>
       <c r="B54" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A54&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Wed</v>
       </c>
       <c r="C54" s="12"/>
@@ -1610,7 +1647,7 @@
         <v>25</v>
       </c>
       <c r="B55" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A55&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Thu</v>
       </c>
       <c r="C55" s="12"/>
@@ -1624,7 +1661,7 @@
         <v>26</v>
       </c>
       <c r="B56" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A56&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Fri</v>
       </c>
       <c r="C56" s="12"/>
@@ -1638,7 +1675,7 @@
         <v>26</v>
       </c>
       <c r="B57" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A57&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Fri</v>
       </c>
       <c r="C57" s="12"/>
@@ -1652,7 +1689,7 @@
         <v>29</v>
       </c>
       <c r="B58" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A58&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Mon</v>
       </c>
       <c r="C58" s="12"/>
@@ -1666,7 +1703,7 @@
         <v>29</v>
       </c>
       <c r="B59" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A59&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Mon</v>
       </c>
       <c r="C59" s="12"/>
@@ -1680,7 +1717,7 @@
         <v>30</v>
       </c>
       <c r="B60" s="11" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A60&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Tue</v>
       </c>
       <c r="C60" s="12"/>
@@ -1694,7 +1731,7 @@
         <v>31</v>
       </c>
       <c r="B61" s="26" t="str">
-        <f>TEXT($B$2&amp;"/"&amp;A61&amp;"/"&amp;$B$1, "ddd")</f>
+        <f t="shared" si="1"/>
         <v>Wed</v>
       </c>
       <c r="C61" s="17"/>
@@ -1708,26 +1745,17 @@
   <mergeCells count="1">
     <mergeCell ref="B3:G3"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{4CA62272-AD96-4093-937E-890B63BDC2C8}">
       <formula1>1</formula1>
       <formula2>12</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G61" xr:uid="{7E79B822-7F4C-473D-94C7-0DD3E57173B1}">
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7E79B822-7F4C-473D-94C7-0DD3E57173B1}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>G61</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>